<commit_message>
add auto connect and update matrix sheet
</commit_message>
<xml_diff>
--- a/features/backlog/android/ServerPage_SymlexVPN.xlsx
+++ b/features/backlog/android/ServerPage_SymlexVPN.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\SymlexVPNTestCases\features\android\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\SymlexVPNTestCases\features\backlog\android\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A715F825-26B4-4988-8ED9-9B4EF5D43E72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70F5B3BF-CAAC-43C5-9243-F6AEA735703D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -617,11 +617,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -641,6 +636,11 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1343,7 +1343,7 @@
   <dimension ref="A1:Z990"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="3" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A19" sqref="A19:G19"/>
     </sheetView>
   </sheetViews>
@@ -1360,15 +1360,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="25" t="s">
         <v>75</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="20"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="27"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
@@ -1390,13 +1390,13 @@
       <c r="Z1" s="1"/>
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="21"/>
-      <c r="B2" s="22"/>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
-      <c r="G2" s="23"/>
+      <c r="A2" s="28"/>
+      <c r="B2" s="29"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="30"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
@@ -1902,25 +1902,25 @@
       <c r="Z14" s="1"/>
     </row>
     <row r="15" spans="1:26" ht="168" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="24" t="s">
+      <c r="A15" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="B15" s="25" t="s">
+      <c r="B15" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="C15" s="24" t="s">
+      <c r="C15" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="D15" s="25" t="s">
+      <c r="D15" s="20" t="s">
         <v>59</v>
       </c>
-      <c r="E15" s="25" t="s">
+      <c r="E15" s="20" t="s">
         <v>60</v>
       </c>
-      <c r="F15" s="26" t="s">
+      <c r="F15" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="G15" s="27"/>
+      <c r="G15" s="22"/>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
@@ -1942,30 +1942,30 @@
       <c r="Z15" s="1"/>
     </row>
     <row r="16" spans="1:26" ht="116.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="24" t="s">
+      <c r="A16" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="B16" s="29" t="s">
+      <c r="B16" s="24" t="s">
         <v>63</v>
       </c>
-      <c r="C16" s="27" t="s">
+      <c r="C16" s="22" t="s">
         <v>62</v>
       </c>
-      <c r="D16" s="29" t="s">
+      <c r="D16" s="24" t="s">
         <v>68</v>
       </c>
-      <c r="E16" s="27" t="s">
+      <c r="E16" s="22" t="s">
         <v>65</v>
       </c>
-      <c r="F16" s="26" t="s">
+      <c r="F16" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="G16" s="27"/>
-      <c r="H16" s="28"/>
-      <c r="I16" s="28"/>
-      <c r="J16" s="28"/>
-      <c r="K16" s="28"/>
-      <c r="L16" s="28"/>
+      <c r="G16" s="22"/>
+      <c r="H16" s="23"/>
+      <c r="I16" s="23"/>
+      <c r="J16" s="23"/>
+      <c r="K16" s="23"/>
+      <c r="L16" s="23"/>
       <c r="M16" s="1"/>
       <c r="N16" s="1"/>
       <c r="O16" s="1"/>

</xml_diff>